<commit_message>
Editing data in this file
</commit_message>
<xml_diff>
--- a/data_files/ETFs_code_selection.xlsx
+++ b/data_files/ETFs_code_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCENI\Engeto\datovaAkademie\ETFs_dashboard\ETFs_dashboard_PowerBI\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380B2780-4FE8-4E8E-9E7D-7971C83DF583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6434025-7556-4CA4-8A48-90EBDA69123E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8207CF75-72B5-4C69-BC21-B93314B60059}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t>SPDR MSCI Europe Materials UCITS ETF</t>
   </si>
@@ -51,34 +51,7 @@
     <t>WKN</t>
   </si>
   <si>
-    <t>replication</t>
-  </si>
-  <si>
-    <t>physical</t>
-  </si>
-  <si>
-    <t>fund size</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>inception date</t>
-  </si>
-  <si>
-    <t>holdings</t>
-  </si>
-  <si>
     <t>basic materials</t>
-  </si>
-  <si>
-    <t>distribution</t>
-  </si>
-  <si>
-    <t>accumulating</t>
   </si>
   <si>
     <t>iShares STOXX Europe 600 Basic Resources UCITS ETF (DE)</t>
@@ -332,12 +305,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -353,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +340,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -676,346 +656,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCCB7BF-F804-436D-BADF-238B9AE2CA91}">
-  <dimension ref="A2:L23"/>
+  <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="59.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2">
-        <v>278000000</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="3">
-        <v>41978</v>
-      </c>
-      <c r="J3">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C15" t="s">
         <v>55</v>
       </c>
-      <c r="E13" t="s">
+      <c r="D15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
         <v>66</v>
       </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E22" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new data files and making adjustments in data_scraper
</commit_message>
<xml_diff>
--- a/data_files/ETFs_code_selection.xlsx
+++ b/data_files/ETFs_code_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCENI\Engeto\datovaAkademie\ETFs_dashboard\ETFs_dashboard_PowerBI\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6434025-7556-4CA4-8A48-90EBDA69123E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA595B3A-BD37-4AC1-AA2F-F0E352FF4277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8207CF75-72B5-4C69-BC21-B93314B60059}"/>
   </bookViews>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCCB7BF-F804-436D-BADF-238B9AE2CA91}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +952,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B19" t="s">

</xml_diff>